<commit_message>
hier_hdbscan expt image and more updates on expt
</commit_message>
<xml_diff>
--- a/Experiments/DBCV_PointNet.xlsx
+++ b/Experiments/DBCV_PointNet.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="117">
   <si>
     <t>Datapoints</t>
   </si>
@@ -362,12 +362,30 @@
   <si>
     <t>19.771 secs</t>
   </si>
+  <si>
+    <t>Nan</t>
+  </si>
+  <si>
+    <t>5683.091 secs</t>
+  </si>
+  <si>
+    <t>71.232 secs</t>
+  </si>
+  <si>
+    <t>181.386 secs</t>
+  </si>
+  <si>
+    <t>TEST DATASET</t>
+  </si>
+  <si>
+    <t>641.189 secs</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,6 +409,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -423,7 +449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -439,6 +465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -744,10 +771,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:N33"/>
+  <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -769,175 +796,74 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="G1" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3">
-        <v>1000</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3">
-        <v>303</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3">
-        <v>512</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="3">
-        <v>2</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-    </row>
-    <row r="3" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3">
-        <v>1000</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="3">
-        <v>169</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="3">
-        <v>512</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3">
-        <v>154</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="1"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-    </row>
-    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>1000</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="3">
-        <v>175</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3">
-        <v>512</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="3">
-        <v>154</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="1"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
     </row>
     <row r="5" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>1000</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3">
-        <v>175</v>
+        <v>303</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="E5" s="3">
         <v>512</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="2"/>
@@ -945,13 +871,13 @@
         <v>2</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -961,33 +887,33 @@
         <v>1000</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C6" s="3">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E6" s="3">
         <v>512</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="3">
-        <v>2</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="G6" s="3">
+        <v>154</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="2"/>
       <c r="K6" s="2" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="M6" s="2"/>
       <c r="N6" s="2"/>
@@ -997,33 +923,33 @@
         <v>1000</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3">
         <v>175</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="E7" s="3">
         <v>512</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>154</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="M7" s="2"/>
       <c r="N7" s="2"/>
@@ -1033,59 +959,55 @@
         <v>1000</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3">
         <v>175</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3">
         <v>512</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G8" s="3">
-        <v>154</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="I8" s="1"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="4" t="s">
-        <v>51</v>
+        <v>32</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="3">
+        <v>2</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>53</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
     </row>
     <row r="9" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>1000</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C9" s="3">
         <v>175</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="E9" s="3">
         <v>512</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="2"/>
@@ -1093,67 +1015,111 @@
         <v>2</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="M9" s="2"/>
       <c r="N9" s="2"/>
     </row>
     <row r="10" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="2"/>
+      <c r="A10" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="3">
+        <v>175</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="3">
+        <v>512</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="3">
+        <v>154</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
+      <c r="K10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="M10" s="2"/>
       <c r="N10" s="2"/>
     </row>
     <row r="11" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="2"/>
+      <c r="A11" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3">
+        <v>175</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="3">
+        <v>512</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11" s="3">
+        <v>154</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="K11" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="C12" s="3">
         <v>175</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E12" s="3">
         <v>512</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="2"/>
@@ -1161,105 +1127,67 @@
         <v>2</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M12" s="2"/>
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3">
-        <v>2000</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C13" s="3">
-        <v>175</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="3">
-        <v>512</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="3">
-        <v>154</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>66</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="2"/>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
-      <c r="K13" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>68</v>
-      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="2"/>
       <c r="M13" s="2"/>
       <c r="N13" s="2"/>
     </row>
     <row r="14" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>2000</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>47</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
       <c r="C14" s="1"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="3">
-        <v>512</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" s="3">
-        <v>154</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>70</v>
-      </c>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="2"/>
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>72</v>
-      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
       <c r="M14" s="2"/>
-      <c r="N14" s="2" t="s">
-        <v>73</v>
-      </c>
+      <c r="N14" s="2"/>
     </row>
     <row r="15" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>2000</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>25</v>
       </c>
       <c r="C15" s="3">
         <v>175</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E15" s="3">
         <v>512</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="2"/>
@@ -1267,13 +1195,13 @@
         <v>2</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>77</v>
+        <v>62</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>78</v>
+        <v>63</v>
       </c>
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
@@ -1283,33 +1211,33 @@
         <v>2000</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="C16" s="3">
-        <v>363</v>
+        <v>175</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="E16" s="3">
         <v>512</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="G16" s="3">
         <v>154</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L16" s="5" t="s">
-        <v>83</v>
+        <v>67</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
@@ -1319,69 +1247,67 @@
         <v>2000</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="3">
-        <v>605</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>84</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
       <c r="E17" s="3">
         <v>512</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="3">
-        <v>2</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>86</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="G17" s="3">
+        <v>154</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="2"/>
       <c r="K17" s="2" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+      <c r="N17" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="18" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>2000</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3">
         <v>175</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="E18" s="3">
         <v>512</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" s="3">
-        <v>154</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="I18" s="1"/>
-      <c r="J18" s="2"/>
+        <v>75</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="3">
+        <v>2</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="K18" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="M18" s="2"/>
       <c r="N18" s="2"/>
@@ -1391,87 +1317,127 @@
         <v>2000</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>14</v>
       </c>
       <c r="C19" s="3">
-        <v>175</v>
+        <v>363</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="E19" s="3">
         <v>512</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="3">
-        <v>2</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>96</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="G19" s="3">
+        <v>154</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="I19" s="1"/>
+      <c r="J19" s="2"/>
       <c r="K19" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="L19" s="2" t="s">
-        <v>98</v>
+        <v>82</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="3">
+        <v>605</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E20" s="3">
+        <v>512</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="G20" s="1"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
+      <c r="I20" s="3">
+        <v>2</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="M20" s="2"/>
       <c r="N20" s="2"/>
     </row>
     <row r="21" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="2"/>
+      <c r="A21" s="3">
+        <v>2000</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="3">
+        <v>175</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" s="3">
+        <v>512</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="3">
+        <v>154</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="I21" s="1"/>
       <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
+      <c r="K21" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>93</v>
+      </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2"/>
     </row>
     <row r="22" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
-        <v>5000</v>
+        <v>2000</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C22" s="3">
-        <v>1586</v>
+        <v>175</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E22" s="3">
         <v>512</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="2"/>
@@ -1479,10 +1445,14 @@
         <v>2</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
+        <v>96</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
@@ -1503,68 +1473,48 @@
       <c r="N23" s="2"/>
     </row>
     <row r="24" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
-        <v>5000</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C24" s="3">
-        <v>175</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="E24" s="3">
-        <v>512</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>103</v>
-      </c>
+      <c r="A24" s="1"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="2"/>
       <c r="G24" s="1"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="3">
-        <v>2</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="L24" s="2" t="s">
-        <v>105</v>
-      </c>
+      <c r="I24" s="1"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
     <row r="25" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
+      <c r="A25" s="3">
         <v>5000</v>
       </c>
-      <c r="B25" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C25" s="1">
-        <v>175</v>
+      <c r="B25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1586</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E25" s="1">
+        <v>99</v>
+      </c>
+      <c r="E25" s="3">
         <v>512</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="G25" s="1">
-        <v>154</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="I25" s="1"/>
-      <c r="J25" s="2"/>
+        <v>100</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="3">
+        <v>2</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
@@ -1587,48 +1537,106 @@
       <c r="N26" s="2"/>
     </row>
     <row r="27" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="2"/>
+      <c r="A27" s="3">
+        <v>5000</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="3">
+        <v>175</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E27" s="3">
+        <v>512</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
+      <c r="I27" s="3">
+        <v>2</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="M27" s="2"/>
       <c r="N27" s="2"/>
     </row>
     <row r="28" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="2"/>
+      <c r="A28" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="1">
+        <v>175</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E28" s="1">
+        <v>512</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G28" s="1">
+        <v>154</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>109</v>
+      </c>
       <c r="I28" s="1"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
+      <c r="K28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="N28" s="2"/>
     </row>
     <row r="29" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="2"/>
+      <c r="A29" s="1">
+        <v>5000</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="1">
+        <v>175</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="1">
+        <v>512</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>113</v>
+      </c>
       <c r="G29" s="1"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="2"/>
+      <c r="I29" s="1">
+        <v>2</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>114</v>
+      </c>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -1683,9 +1691,7 @@
       <c r="N32" s="2"/>
     </row>
     <row r="33" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>106</v>
-      </c>
+      <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
       <c r="D33" s="2"/>
@@ -1700,7 +1706,58 @@
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
     </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="2"/>
+      <c r="N34" s="2"/>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>